<commit_message>
V3 board will fit into the black plastic case 20x28.5mm
</commit_message>
<xml_diff>
--- a/RFID_BOARD_V2_EM4095/BOM_RFID_BOARD_EM4095.xlsx
+++ b/RFID_BOARD_V2_EM4095/BOM_RFID_BOARD_EM4095.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="38320" windowHeight="21760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RFID_BOARD_EM4095.csv" sheetId="1" r:id="rId1"/>
@@ -279,9 +279,6 @@
     <t>placed 10n</t>
   </si>
   <si>
-    <t>placed 10n from würth</t>
-  </si>
-  <si>
     <t>should be 0805 footprint!!!</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>C2012X7T2E104K125AA</t>
+  </si>
+  <si>
+    <t>placed 10n from würth --&gt; Target frequency ca. 124-125 kHz</t>
   </si>
 </sst>
 </file>
@@ -330,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +349,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -364,12 +370,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -705,15 +715,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="28.1640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1185,12 +1195,12 @@
       <c r="H40" t="s">
         <v>17</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I40" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="2">
+      <c r="A41" s="4">
         <v>1</v>
       </c>
       <c r="B41">
@@ -1208,12 +1218,12 @@
       <c r="F41" t="s">
         <v>21</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I41" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="2">
+      <c r="A42" s="4">
         <v>2</v>
       </c>
       <c r="B42">
@@ -1233,7 +1243,7 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>3</v>
       </c>
       <c r="B43">
@@ -1242,7 +1252,7 @@
       <c r="C43" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E43" t="s">
@@ -1256,7 +1266,7 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>4</v>
       </c>
       <c r="B44">
@@ -1274,12 +1284,12 @@
       <c r="F44" t="s">
         <v>24</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="I44" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>5</v>
       </c>
       <c r="B45">
@@ -1299,7 +1309,7 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46">
+      <c r="A46" s="4">
         <v>6</v>
       </c>
       <c r="B46">
@@ -1322,7 +1332,7 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47">
+      <c r="A47" s="5">
         <v>7</v>
       </c>
       <c r="B47">
@@ -1331,7 +1341,7 @@
       <c r="C47" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E47" t="s">
@@ -1341,14 +1351,14 @@
         <v>24</v>
       </c>
       <c r="H47" t="s">
-        <v>90</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="2">
+        <v>89</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="45">
+      <c r="A48" s="1">
         <v>8</v>
       </c>
       <c r="B48">
@@ -1366,12 +1376,12 @@
       <c r="F48" t="s">
         <v>24</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>86</v>
+      <c r="I48" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>9</v>
       </c>
       <c r="B49">
@@ -1380,7 +1390,7 @@
       <c r="C49" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E49" t="s">
@@ -1394,7 +1404,7 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="2">
+      <c r="A50" s="4">
         <v>10</v>
       </c>
       <c r="B50">
@@ -1403,7 +1413,7 @@
       <c r="C50" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E50" t="s">
@@ -1417,7 +1427,7 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="2">
+      <c r="A51" s="4">
         <v>11</v>
       </c>
       <c r="B51">
@@ -1426,7 +1436,7 @@
       <c r="C51" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>52</v>
       </c>
       <c r="E51" t="s">
@@ -1436,11 +1446,11 @@
         <v>24</v>
       </c>
       <c r="H51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="2">
+      <c r="A52" s="4">
         <v>12</v>
       </c>
       <c r="B52">
@@ -1459,8 +1469,14 @@
         <v>56</v>
       </c>
     </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="4"/>
+    </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="2">
+      <c r="A55" s="4">
         <v>15</v>
       </c>
       <c r="B55">
@@ -1480,7 +1496,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="2">
+      <c r="A56" s="4">
         <v>16</v>
       </c>
       <c r="B56">
@@ -1500,7 +1516,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="2">
+      <c r="A57" s="4">
         <v>17</v>
       </c>
       <c r="B57">
@@ -1520,8 +1536,8 @@
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="4" t="s">
-        <v>88</v>
+      <c r="A58" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B58">
         <v>1</v>

</xml_diff>

<commit_message>
panelized v3 RFID PCB
</commit_message>
<xml_diff>
--- a/RFID_BOARD_V2_EM4095/BOM_RFID_BOARD_EM4095.xlsx
+++ b/RFID_BOARD_V2_EM4095/BOM_RFID_BOARD_EM4095.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33520" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RFID_BOARD_EM4095.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="93">
   <si>
     <t>Source:</t>
   </si>
@@ -261,9 +261,6 @@
     <t>C1, C12</t>
   </si>
   <si>
-    <t>C2, C7, C11</t>
-  </si>
-  <si>
     <t>C3, C4, CRES2</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>c1 c11 part value exchanged</t>
   </si>
   <si>
-    <t>placed 10n</t>
-  </si>
-  <si>
     <t>should be 0805 footprint!!!</t>
   </si>
   <si>
@@ -292,13 +286,25 @@
   </si>
   <si>
     <t>placed 10n from würth --&gt; Target frequency ca. 124-125 kHz</t>
+  </si>
+  <si>
+    <t>C2, C7, C8, C11</t>
+  </si>
+  <si>
+    <t>C5 can be max. 22n</t>
+  </si>
+  <si>
+    <t>C5, C6</t>
+  </si>
+  <si>
+    <t>C8 must be precise! The rest is decoupling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,6 +331,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -365,25 +379,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,15 +741,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="28.1640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1195,8 +1221,8 @@
       <c r="H40" t="s">
         <v>17</v>
       </c>
-      <c r="I40" s="6" t="s">
-        <v>83</v>
+      <c r="I40" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1218,19 +1244,19 @@
       <c r="F41" t="s">
         <v>21</v>
       </c>
-      <c r="I41" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="I41" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30">
       <c r="A42" s="4">
         <v>2</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D42" t="s">
         <v>23</v>
@@ -1240,6 +1266,9 @@
       </c>
       <c r="F42" t="s">
         <v>24</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1250,7 +1279,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>26</v>
@@ -1270,13 +1299,13 @@
         <v>4</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
@@ -1284,22 +1313,22 @@
       <c r="F44" t="s">
         <v>24</v>
       </c>
-      <c r="I44" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="I44" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="28" customHeight="1">
       <c r="A45" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
@@ -1307,80 +1336,40 @@
       <c r="F45" t="s">
         <v>24</v>
       </c>
+      <c r="I45" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="4">
-        <v>6</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" s="7" customFormat="1">
+      <c r="A47" s="6">
+        <v>7</v>
+      </c>
+      <c r="B47" s="7">
+        <v>2</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G46" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="5">
-        <v>7</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E47" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" t="s">
-        <v>24</v>
-      </c>
-      <c r="H47" t="s">
-        <v>89</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="45">
-      <c r="A48" s="1">
-        <v>8</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" t="s">
-        <v>43</v>
-      </c>
-      <c r="E48" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" t="s">
-        <v>24</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="H47" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>9</v>
       </c>
@@ -1403,7 +1392,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" s="4">
         <v>10</v>
       </c>
@@ -1426,7 +1415,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:9">
       <c r="A51" s="4">
         <v>11</v>
       </c>
@@ -1446,76 +1435,79 @@
         <v>24</v>
       </c>
       <c r="H51" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="7" customFormat="1">
+      <c r="A52" s="10">
         <v>12</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="7">
         <v>1</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="4"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="4">
+    <row r="55" spans="1:9" s="7" customFormat="1">
+      <c r="A55" s="10">
         <v>15</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="7">
         <v>1</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="4">
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" s="7" customFormat="1">
+      <c r="A56" s="10">
         <v>16</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="7">
         <v>1</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="4">
         <v>17</v>
       </c>
@@ -1535,9 +1527,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:9">
       <c r="A58" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B58">
         <v>1</v>

</xml_diff>

<commit_message>
production status nestbox v3
</commit_message>
<xml_diff>
--- a/RFID_BOARD_V2_EM4095/BOM_RFID_BOARD_EM4095.xlsx
+++ b/RFID_BOARD_V2_EM4095/BOM_RFID_BOARD_EM4095.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33520" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="3680" yWindow="-20" windowWidth="29840" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RFID_BOARD_EM4095.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="FINAL VERSION" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="94">
   <si>
     <t>Source:</t>
   </si>
@@ -298,13 +299,16 @@
   </si>
   <si>
     <t>C8 must be precise! The rest is decoupling</t>
+  </si>
+  <si>
+    <t>(10nF, 50V)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -343,6 +347,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -370,7 +380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -378,16 +388,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -403,13 +430,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,14 +776,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView topLeftCell="A38" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="9" max="9" width="28.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1556,4 +1592,311 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="4.5" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="33" customHeight="1">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>4</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="87" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
various changes & updates, production state
</commit_message>
<xml_diff>
--- a/RFID_BOARD_V2_EM4095/BOM_RFID_BOARD_EM4095.xlsx
+++ b/RFID_BOARD_V2_EM4095/BOM_RFID_BOARD_EM4095.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffael/Desktop/Octanis/Octanis3/pcb/RFID_BOARD_V2_EM4095/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246F2EC6-FFCC-AC44-AE72-B65CFA78541E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="-20" windowWidth="29840" windowHeight="20540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33580" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RFID_BOARD_EM4095.csv" sheetId="1" r:id="rId1"/>
     <sheet name="FINAL VERSION" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="110">
   <si>
     <t>Source:</t>
   </si>
@@ -301,14 +307,62 @@
     <t>C8 must be precise! The rest is decoupling</t>
   </si>
   <si>
-    <t>(10nF, 50V)</t>
+    <t>res3</t>
+  </si>
+  <si>
+    <t>res2</t>
+  </si>
+  <si>
+    <t>res1</t>
+  </si>
+  <si>
+    <t>capacitor choice (nF)</t>
+  </si>
+  <si>
+    <t>f_res (kHz)</t>
+  </si>
+  <si>
+    <t>Inductor value</t>
+  </si>
+  <si>
+    <t>VJ0603Y153JXAAC</t>
+  </si>
+  <si>
+    <t>CC0805JKNPOBBN102</t>
+  </si>
+  <si>
+    <t>(C0805C102JAGACTU or CC0805JKNPOBBN102)</t>
+  </si>
+  <si>
+    <t>CGA3E1C0G2A103J080AC</t>
+  </si>
+  <si>
+    <t>GRM21BR61E106MA73L</t>
+  </si>
+  <si>
+    <t>GCM188L81H104KA57D</t>
+  </si>
+  <si>
+    <t>C5 can be max. 22n, alternative: GRM1885C1H103JA01D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8 </t>
+  </si>
+  <si>
+    <t>100n 1%</t>
+  </si>
+  <si>
+    <t>12nF</t>
+  </si>
+  <si>
+    <t>15n alternative: VJ0603Y153JXAAC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,8 +407,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,8 +439,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -403,8 +487,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -413,8 +508,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -435,9 +531,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -445,10 +547,19 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -773,14 +884,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView topLeftCell="A38" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -788,7 +899,7 @@
     <col min="9" max="9" width="28.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -796,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -804,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -812,7 +923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -820,7 +931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -828,12 +939,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -859,7 +970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>18</v>
       </c>
@@ -873,7 +984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>22</v>
       </c>
@@ -887,7 +998,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>25</v>
       </c>
@@ -904,7 +1015,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>28</v>
       </c>
@@ -921,7 +1032,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>29</v>
       </c>
@@ -935,7 +1046,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>31</v>
       </c>
@@ -949,7 +1060,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>33</v>
       </c>
@@ -963,7 +1074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="3:8">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>34</v>
       </c>
@@ -980,7 +1091,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="3:8">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>37</v>
       </c>
@@ -994,7 +1105,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="3:8">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>39</v>
       </c>
@@ -1008,7 +1119,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="3:8">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>40</v>
       </c>
@@ -1022,7 +1133,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="3:8">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>41</v>
       </c>
@@ -1036,7 +1147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="3:8">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>42</v>
       </c>
@@ -1050,7 +1161,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="3:8">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>44</v>
       </c>
@@ -1067,7 +1178,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="3:8">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>45</v>
       </c>
@@ -1084,7 +1195,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="3:8">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>48</v>
       </c>
@@ -1101,7 +1212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="3:8">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>51</v>
       </c>
@@ -1115,7 +1226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="3:8">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>53</v>
       </c>
@@ -1129,7 +1240,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="3:8">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>57</v>
       </c>
@@ -1143,7 +1254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="3:8">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>61</v>
       </c>
@@ -1157,7 +1268,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="3:8">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>65</v>
       </c>
@@ -1171,7 +1282,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="3:8">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>66</v>
       </c>
@@ -1185,7 +1296,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="3:8">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>70</v>
       </c>
@@ -1199,7 +1310,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>72</v>
       </c>
@@ -1213,7 +1324,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>74</v>
       </c>
@@ -1227,12 +1338,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1261,7 +1372,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>1</v>
       </c>
@@ -1284,7 +1395,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30">
+    <row r="42" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>2</v>
       </c>
@@ -1307,7 +1418,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>3</v>
       </c>
@@ -1330,7 +1441,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>4</v>
       </c>
@@ -1353,7 +1464,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="28" customHeight="1">
+    <row r="45" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>8</v>
       </c>
@@ -1376,10 +1487,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" spans="1:9" s="7" customFormat="1">
+    <row r="47" spans="1:9" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>7</v>
       </c>
@@ -1405,7 +1516,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>9</v>
       </c>
@@ -1428,7 +1539,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>10</v>
       </c>
@@ -1451,7 +1562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>11</v>
       </c>
@@ -1474,7 +1585,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="7" customFormat="1">
+    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="10">
         <v>12</v>
       </c>
@@ -1495,13 +1606,13 @@
       </c>
       <c r="I52" s="9"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:9" s="7" customFormat="1">
+    <row r="55" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="10">
         <v>15</v>
       </c>
@@ -1522,7 +1633,7 @@
       </c>
       <c r="I55" s="9"/>
     </row>
-    <row r="56" spans="1:9" s="7" customFormat="1">
+    <row r="56" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="10">
         <v>16</v>
       </c>
@@ -1543,7 +1654,7 @@
       </c>
       <c r="I56" s="9"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>17</v>
       </c>
@@ -1563,7 +1674,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>85</v>
       </c>
@@ -1595,28 +1706,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I11"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="2" max="2" width="4.5" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="30.83203125" customWidth="1"/>
+    <col min="9" max="9" width="39.83203125" customWidth="1"/>
     <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -1644,8 +1756,11 @@
       <c r="I1" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1655,7 +1770,7 @@
       <c r="C2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="18" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -1665,10 +1780,30 @@
         <v>21</v>
       </c>
       <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="H2" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1">
+      <c r="J2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2">
+        <v>2.8</v>
+      </c>
+      <c r="L2">
+        <v>2.56</v>
+      </c>
+      <c r="M2">
+        <v>2.56</v>
+      </c>
+      <c r="N2">
+        <v>2.56</v>
+      </c>
+      <c r="O2">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1678,7 +1813,7 @@
       <c r="C3" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -1688,73 +1823,104 @@
         <v>24</v>
       </c>
       <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="H3" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="I3" s="12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="13">
+      <c r="J3" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N3" s="15">
+        <v>1</v>
+      </c>
+      <c r="O3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="14"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
-        <v>3</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="13">
+      <c r="I5" s="12"/>
+      <c r="J5" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K5">
+        <v>1.8</v>
+      </c>
+      <c r="L5">
+        <v>1.8</v>
+      </c>
+      <c r="M5">
+        <v>1.6</v>
+      </c>
+      <c r="N5" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="O5" s="15">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B6" s="11">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D6" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30">
-      <c r="A6" s="13">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>20</v>
@@ -1763,48 +1929,93 @@
         <v>24</v>
       </c>
       <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="H6" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="I6" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>105</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6" s="15">
+        <v>15</v>
+      </c>
+      <c r="O6" s="15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7">
+        <f>0.001/(2*PI()*SQRT(K2/1000/(1000000000/K3+1000000000/K5+1000000000/K6)))</f>
+        <v>122.38071760849164</v>
+      </c>
+      <c r="L7">
+        <f>0.001/(2*PI()*SQRT(L2/1000/(1000000000/L3+1000000000/L5+1000000000/L6)))</f>
+        <v>127.98881805197479</v>
+      </c>
+      <c r="M7">
+        <f>0.001/(2*PI()*SQRT(M2/1000/(1000000000/M3+1000000000/M5+1000000000/M6)))</f>
+        <v>127.15640939420561</v>
+      </c>
+      <c r="N7">
+        <f>0.001/(2*PI()*SQRT(N2/1000/(1000000000/N3+1000000000/N5+1000000000/N6)))</f>
+        <v>126.69378826527277</v>
+      </c>
+      <c r="O7">
+        <f>0.001/(2*PI()*SQRT(O2/1000/(1000000000/O3+1000000000/O5+1000000000/O6)))</f>
+        <v>124.64823454300625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D8" s="19" t="s">
         <v>46</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="13">
-        <v>7</v>
-      </c>
-      <c r="B8" s="11">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>20</v>
@@ -1813,84 +2024,114 @@
         <v>21</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="H8" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="11">
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="13">
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
-        <v>1</v>
-      </c>
-      <c r="C10" s="11" t="s">
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="13">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="12"/>
     </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H7" r:id="rId1" display="https://www.mouser.ch/ProductDetail/Vishay-Vitramon/VJ0603Y153JXAAC?qs=sGAEpiMZZMs0AnBnWHyRQKubRBCdVSJlEvhtpSFB550%3d" xr:uid="{925002C3-1114-FD45-852F-CF0A8E88EBF5}"/>
+  </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="87" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>